<commit_message>
T6B - dados da aula
</commit_message>
<xml_diff>
--- a/T6B - lançamento.xlsx
+++ b/T6B - lançamento.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nunop\OneDrive\Ambiente de Trabalho\6b - lançamento\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nunop\OneDrive\Documentos\GitHub\LABSFISICAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E43D86C-EED5-4391-B24F-33C9F538C0F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9537EE2E-F34D-46FE-AB47-5090D401E892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E3B97DAB-F56B-4F1D-B140-62E03DA4F1DE}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Ensaio</t>
   </si>
@@ -71,30 +71,6 @@
   </si>
   <si>
     <r>
-      <t>u(x</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>̄)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (m)</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>v</t>
     </r>
     <r>
@@ -126,32 +102,6 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> (m/s)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>u(v̄</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>o</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>) (m/s)</t>
     </r>
   </si>
   <si>
@@ -299,13 +249,70 @@
   <si>
     <t>v0 ajuste</t>
   </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>2.292</t>
+  </si>
+  <si>
+    <r>
+      <t>u(x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>̄)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (%)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>u(v̄</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>o</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) (%)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000%"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -429,15 +436,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -446,12 +450,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -466,6 +464,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -475,9 +477,20 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -591,25 +604,25 @@
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1.8897999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>2.1025</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2.2114000000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2.2917999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>2.2842500000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>2.2054999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>2.0489999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1229,25 +1242,25 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="7"/>
                   <c:pt idx="0">
-                    <c:v>0</c:v>
+                    <c:v>8.8035259253614281E-4</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0</c:v>
+                    <c:v>9.340931402172511E-4</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0</c:v>
+                    <c:v>4.3450448817304913E-4</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0</c:v>
+                    <c:v>3.0462570863840831E-4</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0</c:v>
+                    <c:v>3.4528351233845459E-4</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0</c:v>
+                    <c:v>2.9880250536553759E-4</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0</c:v>
+                    <c:v>1.2092481180662877E-3</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1259,25 +1272,25 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="7"/>
                   <c:pt idx="0">
-                    <c:v>0</c:v>
+                    <c:v>8.8035259253614281E-4</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0</c:v>
+                    <c:v>9.340931402172511E-4</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0</c:v>
+                    <c:v>4.3450448817304913E-4</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0</c:v>
+                    <c:v>3.0462570863840831E-4</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0</c:v>
+                    <c:v>3.4528351233845459E-4</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0</c:v>
+                    <c:v>2.9880250536553759E-4</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0</c:v>
+                    <c:v>1.2092481180662877E-3</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1333,25 +1346,25 @@
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>4.6267614688440091</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>4.685000026749865</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>4.6934524986870576</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>4.7415775855721272</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>4.7701341298481461</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>4.798385394827001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>4.8177045950114499</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2006,25 +2019,25 @@
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1.8897999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>2.1025</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2.2114000000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2.2917999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>2.2842500000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>2.2054999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>2.0489999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5551,159 +5564,232 @@
   <dimension ref="A1:M38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="9" max="9" width="9.77734375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="7"/>
-      <c r="B1" s="7" t="s">
+      <c r="A1" s="17"/>
+      <c r="B1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="8">
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="6">
         <v>10</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="6">
         <v>20</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="6">
         <v>30</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="6">
         <v>35</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="6">
         <v>40</v>
       </c>
-      <c r="H2" s="8">
+      <c r="H2" s="6">
         <v>45</v>
       </c>
-      <c r="I2" s="8">
+      <c r="I2" s="6">
         <v>50</v>
       </c>
-      <c r="J2" s="8">
+      <c r="J2" s="6">
         <v>55</v>
       </c>
-      <c r="K2" s="8">
+      <c r="K2" s="6">
         <v>60</v>
       </c>
-      <c r="L2" s="8">
+      <c r="L2" s="6">
         <v>70</v>
       </c>
-      <c r="M2" s="8">
+      <c r="M2" s="6">
         <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="6">
         <v>1</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
+      <c r="E3" s="2">
+        <v>1.8819999999999999</v>
+      </c>
+      <c r="F3" s="2">
+        <v>2.109</v>
+      </c>
+      <c r="G3" s="2">
+        <v>2.2029999999999998</v>
+      </c>
+      <c r="H3" s="2">
+        <v>2.29</v>
+      </c>
+      <c r="I3" s="2">
+        <v>2.2869999999999999</v>
+      </c>
+      <c r="J3" s="2">
+        <v>2.2109999999999999</v>
+      </c>
+      <c r="K3" s="2">
+        <v>2.0129999999999999</v>
+      </c>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="7"/>
-      <c r="B4" s="8">
+      <c r="A4" s="17"/>
+      <c r="B4" s="6">
         <v>2</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
+      <c r="E4" s="2">
+        <v>1.877</v>
+      </c>
+      <c r="F4" s="2">
+        <v>2.0790000000000002</v>
+      </c>
+      <c r="G4" s="2">
+        <v>2.2010000000000001</v>
+      </c>
+      <c r="H4" s="2">
+        <v>2.302</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="K4" s="2">
+        <v>2.0710000000000002</v>
+      </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8">
+      <c r="A5" s="17"/>
+      <c r="B5" s="6">
         <v>3</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
+      <c r="E5" s="2">
+        <v>1.913</v>
+      </c>
+      <c r="F5" s="2">
+        <v>2.1179999999999999</v>
+      </c>
+      <c r="G5" s="2">
+        <v>2.2130000000000001</v>
+      </c>
+      <c r="H5" s="2">
+        <v>2.2959999999999998</v>
+      </c>
+      <c r="I5" s="2">
+        <v>2.2850000000000001</v>
+      </c>
+      <c r="J5" s="2">
+        <v>2.2094999999999998</v>
+      </c>
+      <c r="K5" s="2">
+        <v>2.0619999999999998</v>
+      </c>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="7"/>
-      <c r="B6" s="8">
+      <c r="A6" s="17"/>
+      <c r="B6" s="6">
         <v>4</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
+      <c r="E6" s="2">
+        <v>1.885</v>
+      </c>
+      <c r="F6" s="2">
+        <v>2.0870000000000002</v>
+      </c>
+      <c r="G6" s="2">
+        <v>2.2240000000000002</v>
+      </c>
+      <c r="H6" s="2">
+        <v>2.286</v>
+      </c>
+      <c r="I6" s="2">
+        <v>2.2730000000000001</v>
+      </c>
+      <c r="J6" s="2">
+        <v>2.1970000000000001</v>
+      </c>
+      <c r="K6" s="2">
+        <v>2.0569999999999999</v>
+      </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="7"/>
-      <c r="B7" s="8">
+      <c r="A7" s="17"/>
+      <c r="B7" s="6">
         <v>5</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
+      <c r="E7" s="2">
+        <v>1.8919999999999999</v>
+      </c>
+      <c r="F7" s="2">
+        <v>2.1194999999999999</v>
+      </c>
+      <c r="G7" s="2">
+        <v>2.2160000000000002</v>
+      </c>
+      <c r="H7" s="2">
+        <v>2.2850000000000001</v>
+      </c>
+      <c r="I7" s="2">
+        <v>2.2919999999999998</v>
+      </c>
+      <c r="J7" s="2">
+        <v>2.21</v>
+      </c>
+      <c r="K7" s="2">
+        <v>2.0419999999999998</v>
+      </c>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="7"/>
+      <c r="B8" s="17"/>
       <c r="C8" s="2" t="e">
         <f>AVERAGE(C3:C7)</f>
         <v>#DIV/0!</v>
@@ -5712,33 +5798,33 @@
         <f t="shared" ref="D8:M8" si="0">AVERAGE(D3:D7)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E8" s="2" t="e">
+      <c r="E8" s="2">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F8" s="2" t="e">
+        <v>1.8897999999999999</v>
+      </c>
+      <c r="F8" s="2">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G8" s="2" t="e">
+        <v>2.1025</v>
+      </c>
+      <c r="G8" s="2">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H8" s="2" t="e">
+        <v>2.2114000000000003</v>
+      </c>
+      <c r="H8" s="2">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I8" s="2" t="e">
+        <v>2.2917999999999998</v>
+      </c>
+      <c r="I8" s="2">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J8" s="2" t="e">
+        <v>2.2842500000000001</v>
+      </c>
+      <c r="J8" s="2">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K8" s="2" t="e">
+        <v>2.2054999999999998</v>
+      </c>
+      <c r="K8" s="2">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>2.0489999999999999</v>
       </c>
       <c r="L8" s="2" t="e">
         <f t="shared" si="0"/>
@@ -5750,10 +5836,10 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="7"/>
+      <c r="A9" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="17"/>
       <c r="C9" s="2" t="e">
         <f>STDEV(C3:C7)</f>
         <v>#DIV/0!</v>
@@ -5762,33 +5848,33 @@
         <f t="shared" ref="D9:M9" si="1">STDEV(D3:D7)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E9" s="2" t="e">
+      <c r="E9" s="2">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F9" s="2" t="e">
+        <v>1.4060583202698268E-2</v>
+      </c>
+      <c r="F9" s="2">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G9" s="2" t="e">
+        <v>1.8466185312619253E-2</v>
+      </c>
+      <c r="G9" s="2">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H9" s="2" t="e">
+        <v>9.5026312145637878E-3</v>
+      </c>
+      <c r="H9" s="2">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I9" s="2" t="e">
+        <v>7.1554175279992735E-3</v>
+      </c>
+      <c r="I9" s="2">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J9" s="2" t="e">
+        <v>8.0570879768477564E-3</v>
+      </c>
+      <c r="J9" s="2">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K9" s="2" t="e">
+        <v>6.4999999999998739E-3</v>
+      </c>
+      <c r="K9" s="2">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>2.2704625079485525E-2</v>
       </c>
       <c r="L9" s="2" t="e">
         <f t="shared" si="1"/>
@@ -5800,60 +5886,60 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="3" t="e">
-        <f>C9/SQRT(5)</f>
+      <c r="A10" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="17"/>
+      <c r="C10" s="18" t="e">
+        <f>(C9/SQRT(5))/C8</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D10" s="3" t="e">
-        <f t="shared" ref="D10:M10" si="2">D9/SQRT(5)</f>
+      <c r="D10" s="18" t="e">
+        <f t="shared" ref="D10:M10" si="2">(D9/SQRT(5))/D8</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E10" s="3" t="e">
+      <c r="E10" s="18">
+        <f t="shared" si="2"/>
+        <v>3.3273806587496061E-3</v>
+      </c>
+      <c r="F10" s="18">
+        <f t="shared" si="2"/>
+        <v>3.9278616546135408E-3</v>
+      </c>
+      <c r="G10" s="18">
+        <f t="shared" si="2"/>
+        <v>1.9217264502917623E-3</v>
+      </c>
+      <c r="H10" s="18">
+        <f t="shared" si="2"/>
+        <v>1.3962823981150084E-3</v>
+      </c>
+      <c r="I10" s="18">
+        <f t="shared" si="2"/>
+        <v>1.5774277261182299E-3</v>
+      </c>
+      <c r="J10" s="18">
+        <f t="shared" si="2"/>
+        <v>1.3180178511673862E-3</v>
+      </c>
+      <c r="K10" s="18">
+        <f t="shared" si="2"/>
+        <v>4.9554987878356466E-3</v>
+      </c>
+      <c r="L10" s="18" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F10" s="3" t="e">
+      <c r="M10" s="18" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G10" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H10" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I10" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J10" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K10" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L10" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M10" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
     </row>
     <row r="11" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="7"/>
+      <c r="A11" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="17"/>
       <c r="C11" s="2" t="e">
         <f>SQRT($B$16*C8/C13)</f>
         <v>#DIV/0!</v>
@@ -5862,33 +5948,33 @@
         <f t="shared" ref="D11:M11" si="3">SQRT($B$16*D8/D13)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E11" s="2" t="e">
+      <c r="E11" s="2">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F11" s="2" t="e">
+        <v>4.6267614688440091</v>
+      </c>
+      <c r="F11" s="2">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G11" s="2" t="e">
+        <v>4.685000026749865</v>
+      </c>
+      <c r="G11" s="2">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H11" s="2" t="e">
+        <v>4.6934524986870576</v>
+      </c>
+      <c r="H11" s="2">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I11" s="2" t="e">
+        <v>4.7415775855721272</v>
+      </c>
+      <c r="I11" s="2">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J11" s="2" t="e">
+        <v>4.7701341298481461</v>
+      </c>
+      <c r="J11" s="2">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K11" s="2" t="e">
+        <v>4.798385394827001</v>
+      </c>
+      <c r="K11" s="2">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>4.8177045950114499</v>
       </c>
       <c r="L11" s="2" t="e">
         <f t="shared" si="3"/>
@@ -5900,60 +5986,60 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="2" t="e">
-        <f>1/2*C10*SQRT($B$16/(C13*C8))</f>
+      <c r="A12" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="17"/>
+      <c r="C12" s="19" t="e">
+        <f>(1/2*C10*SQRT($B$16/(C13*C8)))/C11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D12" s="2" t="e">
-        <f t="shared" ref="D12:M12" si="4">1/2*D10*SQRT($B$16/(D13*D8))</f>
+      <c r="D12" s="19" t="e">
+        <f t="shared" ref="D12:M12" si="4">(1/2*D10*SQRT($B$16/(D13*D8)))/D11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E12" s="2" t="e">
+      <c r="E12" s="19">
+        <f t="shared" si="4"/>
+        <v>8.8035259253614281E-4</v>
+      </c>
+      <c r="F12" s="19">
+        <f t="shared" si="4"/>
+        <v>9.340931402172511E-4</v>
+      </c>
+      <c r="G12" s="19">
+        <f t="shared" si="4"/>
+        <v>4.3450448817304913E-4</v>
+      </c>
+      <c r="H12" s="20">
+        <f t="shared" si="4"/>
+        <v>3.0462570863840831E-4</v>
+      </c>
+      <c r="I12" s="20">
+        <f t="shared" si="4"/>
+        <v>3.4528351233845459E-4</v>
+      </c>
+      <c r="J12" s="19">
+        <f t="shared" si="4"/>
+        <v>2.9880250536553759E-4</v>
+      </c>
+      <c r="K12" s="19">
+        <f t="shared" si="4"/>
+        <v>1.2092481180662877E-3</v>
+      </c>
+      <c r="L12" s="19" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F12" s="2" t="e">
+      <c r="M12" s="19" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G12" s="2" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H12" s="2" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I12" s="2" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J12" s="2" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K12" s="2" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L12" s="2" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M12" s="2" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="7"/>
+      <c r="A13" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="17"/>
       <c r="C13" s="2">
         <f>SIN(2*PI()*C2/180)</f>
         <v>0.34202014332566871</v>
@@ -6000,8 +6086,8 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="s">
-        <v>10</v>
+      <c r="A16" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="B16" s="1">
         <v>9.81</v>
@@ -6009,31 +6095,31 @@
     </row>
     <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="16"/>
+      <c r="A18" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="15"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" s="4" t="e">
+      <c r="A19" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="3" t="e">
         <f t="array" ref="B19:C21">LINEST(C8:M8,C13:M13,1,1)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C19" s="4" t="e">
+      <c r="C19" s="3" t="e">
         <v>#VALUE!</v>
       </c>
-      <c r="D19" s="12" t="s">
-        <v>11</v>
+      <c r="D19" s="9" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="11" t="s">
-        <v>15</v>
+      <c r="A20" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="B20" s="1" t="e">
         <v>#VALUE!</v>
@@ -6041,13 +6127,13 @@
       <c r="C20" s="1" t="e">
         <v>#VALUE!</v>
       </c>
-      <c r="D20" s="13" t="s">
-        <v>12</v>
+      <c r="D20" s="10" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="11" t="s">
-        <v>14</v>
+      <c r="A21" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="B21" s="1" t="e">
         <v>#VALUE!</v>
@@ -6055,140 +6141,143 @@
       <c r="C21" s="1" t="e">
         <v>#VALUE!</v>
       </c>
-      <c r="D21" s="13" t="s">
-        <v>13</v>
+      <c r="D21" s="10" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B25" s="5" t="e">
+      <c r="A25" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="4">
         <f>AVERAGEA(E11:K11)</f>
-        <v>#DIV/0!</v>
+        <v>4.7332879570770938</v>
+      </c>
+      <c r="D25" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27" s="5" t="e">
+      <c r="A27" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" s="4">
         <f>STDEV(E11:K11)</f>
-        <v>#DIV/0!</v>
+        <v>6.8382117796380384E-2</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B29" s="5" t="e">
+      <c r="A29" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" s="4">
         <f>B27/SQRT(7)</f>
-        <v>#DIV/0!</v>
+        <v>2.584601111616381E-2</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A33" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B33" s="18"/>
-      <c r="C33" s="5" t="e">
+      <c r="A33" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33" s="12"/>
+      <c r="C33" s="4" t="e">
         <f>$B$19*C13+$C$19</f>
         <v>#VALUE!</v>
       </c>
-      <c r="D33" s="5" t="e">
+      <c r="D33" s="4" t="e">
         <f t="shared" ref="D33:M33" si="6">$B$19*D13+$C$19</f>
         <v>#VALUE!</v>
       </c>
-      <c r="E33" s="5" t="e">
+      <c r="E33" s="4" t="e">
         <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F33" s="5" t="e">
+      <c r="F33" s="4" t="e">
         <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G33" s="5" t="e">
+      <c r="G33" s="4" t="e">
         <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
-      <c r="H33" s="5" t="e">
+      <c r="H33" s="4" t="e">
         <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
-      <c r="I33" s="5" t="e">
+      <c r="I33" s="4" t="e">
         <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
-      <c r="J33" s="5" t="e">
+      <c r="J33" s="4" t="e">
         <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
-      <c r="K33" s="5" t="e">
+      <c r="K33" s="4" t="e">
         <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
-      <c r="L33" s="5" t="e">
+      <c r="L33" s="4" t="e">
         <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
-      <c r="M33" s="5" t="e">
+      <c r="M33" s="4" t="e">
         <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A34" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B34" s="18"/>
-      <c r="C34" s="6" t="e">
+      <c r="A34" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34" s="12"/>
+      <c r="C34" s="5" t="e">
         <f>C8-C33</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D34" s="6" t="e">
+      <c r="D34" s="5" t="e">
         <f t="shared" ref="D34:M34" si="7">D8-D33</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E34" s="6" t="e">
+      <c r="E34" s="5" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F34" s="5" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G34" s="5" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H34" s="5" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I34" s="5" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J34" s="5" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K34" s="5" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L34" s="5" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F34" s="6" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G34" s="6" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H34" s="6" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I34" s="6" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J34" s="6" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K34" s="6" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L34" s="6" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M34" s="6" t="e">
+      <c r="M34" s="5" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="K38" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L38" t="e">
         <f>SQRT(B16*B19)</f>

</xml_diff>